<commit_message>
updated payoffs & belief screen in 2 projects app
</commit_message>
<xml_diff>
--- a/pilot_2_projects/static/Parameters.xlsx
+++ b/pilot_2_projects/static/Parameters.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frauke/GithubRepoTree/pilot_2_projects/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C463238-2D3E-B041-96D4-2362A062A29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A870C47-3198-C141-9B53-DB313CB77BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AD373C2C-5915-3449-9931-3E1FB904DA92}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AD373C2C-5915-3449-9931-3E1FB904DA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>efficiency_A</t>
   </si>
@@ -58,6 +58,42 @@
   </si>
   <si>
     <t>num_X_B</t>
+  </si>
+  <si>
+    <t>image_title_A</t>
+  </si>
+  <si>
+    <t>image_title_B</t>
+  </si>
+  <si>
+    <t>matrix_60.png</t>
+  </si>
+  <si>
+    <t>matrix_80.png</t>
+  </si>
+  <si>
+    <t>matrix_100.png</t>
+  </si>
+  <si>
+    <t>matrix_120.png</t>
+  </si>
+  <si>
+    <t>matrix_160.png</t>
+  </si>
+  <si>
+    <t>matrix_200.png</t>
+  </si>
+  <si>
+    <t>matrix_300.png</t>
+  </si>
+  <si>
+    <t>matrix_340.png</t>
+  </si>
+  <si>
+    <t>matrix_320.png</t>
+  </si>
+  <si>
+    <t>matrix_280.png</t>
   </si>
 </sst>
 </file>
@@ -80,12 +116,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,12 +142,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -422,15 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CB44EE-A13A-B449-954A-F65A63BC6646}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H10"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,19 +489,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1.5</v>
       </c>
@@ -469,20 +520,26 @@
       <c r="D2" s="1">
         <v>60</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
         <v>2.125</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>34</v>
       </c>
-      <c r="G2" s="1">
-        <v>16</v>
-      </c>
       <c r="H2" s="1">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1">
         <v>340</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -495,20 +552,26 @@
       <c r="D3" s="1">
         <v>80</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>32</v>
       </c>
-      <c r="G3" s="1">
-        <v>16</v>
-      </c>
       <c r="H3" s="1">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1">
         <v>320</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2.5</v>
       </c>
@@ -521,173 +584,215 @@
       <c r="D4" s="1">
         <v>100</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1">
         <v>1.875</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>30</v>
       </c>
-      <c r="G4" s="1">
-        <v>16</v>
-      </c>
       <c r="H4" s="1">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="G5" s="1">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1">
+        <v>280</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>2.5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
         <v>100</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.625</v>
       </c>
-      <c r="F5" s="1">
-        <v>28</v>
-      </c>
-      <c r="G5" s="1">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="G6" s="1">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1">
+        <v>100</v>
+      </c>
+      <c r="J6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>120</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1.75</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="1">
+        <v>200</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1">
+        <v>200</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>300</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.875</v>
+      </c>
+      <c r="G8" s="1">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2">
+        <v>16</v>
+      </c>
+      <c r="I8" s="1">
+        <v>300</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
         <v>160</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2">
-        <v>16</v>
-      </c>
-      <c r="H7" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="G9" s="1">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
+        <v>80</v>
+      </c>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="1">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="B10" s="1">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1">
         <v>160</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="1">
-        <v>30</v>
-      </c>
-      <c r="G8" s="2">
-        <v>16</v>
-      </c>
-      <c r="H8" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1">
-        <v>200</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="F9" s="1">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1">
-        <v>4</v>
-      </c>
-      <c r="H9" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="B10" s="1">
-        <v>30</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1">
-        <v>300</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1.875</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>32</v>
       </c>
-      <c r="G10" s="1">
-        <v>16</v>
-      </c>
       <c r="H10" s="1">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1">
         <v>320</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated belief page design
</commit_message>
<xml_diff>
--- a/pilot_2_projects/static/Parameters.xlsx
+++ b/pilot_2_projects/static/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frauke/GithubRepoTree/pilot_2_projects/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A870C47-3198-C141-9B53-DB313CB77BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FC0757-FEC4-FC45-8174-8BDE8884DF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AD373C2C-5915-3449-9931-3E1FB904DA92}"/>
   </bookViews>
@@ -36,6 +36,36 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
+    <t>matrix_60.png</t>
+  </si>
+  <si>
+    <t>matrix_80.png</t>
+  </si>
+  <si>
+    <t>matrix_100.png</t>
+  </si>
+  <si>
+    <t>matrix_120.png</t>
+  </si>
+  <si>
+    <t>matrix_160.png</t>
+  </si>
+  <si>
+    <t>matrix_200.png</t>
+  </si>
+  <si>
+    <t>matrix_300.png</t>
+  </si>
+  <si>
+    <t>matrix_340.png</t>
+  </si>
+  <si>
+    <t>matrix_320.png</t>
+  </si>
+  <si>
+    <t>matrix_280.png</t>
+  </si>
+  <si>
     <t>efficiency_A</t>
   </si>
   <si>
@@ -48,6 +78,9 @@
     <t>num_X_A</t>
   </si>
   <si>
+    <t>image_title_A</t>
+  </si>
+  <si>
     <t>efficiency_B</t>
   </si>
   <si>
@@ -60,40 +93,7 @@
     <t>num_X_B</t>
   </si>
   <si>
-    <t>image_title_A</t>
-  </si>
-  <si>
     <t>image_title_B</t>
-  </si>
-  <si>
-    <t>matrix_60.png</t>
-  </si>
-  <si>
-    <t>matrix_80.png</t>
-  </si>
-  <si>
-    <t>matrix_100.png</t>
-  </si>
-  <si>
-    <t>matrix_120.png</t>
-  </si>
-  <si>
-    <t>matrix_160.png</t>
-  </si>
-  <si>
-    <t>matrix_200.png</t>
-  </si>
-  <si>
-    <t>matrix_300.png</t>
-  </si>
-  <si>
-    <t>matrix_340.png</t>
-  </si>
-  <si>
-    <t>matrix_320.png</t>
-  </si>
-  <si>
-    <t>matrix_280.png</t>
   </si>
 </sst>
 </file>
@@ -470,41 +470,41 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -521,7 +521,7 @@
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>2.125</v>
@@ -536,7 +536,7 @@
         <v>340</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -553,7 +553,7 @@
         <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -568,7 +568,7 @@
         <v>320</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -585,7 +585,7 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1">
         <v>1.875</v>
@@ -600,7 +600,7 @@
         <v>300</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -617,7 +617,7 @@
         <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F5" s="3">
         <v>1.75</v>
@@ -632,7 +632,7 @@
         <v>280</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -649,7 +649,7 @@
         <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
         <v>0.625</v>
@@ -664,7 +664,7 @@
         <v>100</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -681,7 +681,7 @@
         <v>200</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
         <v>1.25</v>
@@ -696,7 +696,7 @@
         <v>200</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>300</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1">
         <v>1.875</v>
@@ -728,7 +728,7 @@
         <v>300</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
         <v>160</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
@@ -760,7 +760,7 @@
         <v>80</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -777,7 +777,7 @@
         <v>160</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -792,7 +792,7 @@
         <v>320</v>
       </c>
       <c r="J10" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
randomized left and right order
</commit_message>
<xml_diff>
--- a/pilot_2_projects/static/Parameters.xlsx
+++ b/pilot_2_projects/static/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frauke/GithubRepoTree/pilot_2_projects/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FC0757-FEC4-FC45-8174-8BDE8884DF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A626F5C-61E6-F54C-AE3A-9425D62EF12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AD373C2C-5915-3449-9931-3E1FB904DA92}"/>
   </bookViews>
@@ -66,34 +66,34 @@
     <t>matrix_280.png</t>
   </si>
   <si>
-    <t>efficiency_A</t>
-  </si>
-  <si>
-    <t>num_doses_A</t>
-  </si>
-  <si>
-    <t>price_A</t>
-  </si>
-  <si>
-    <t>num_X_A</t>
-  </si>
-  <si>
-    <t>image_title_A</t>
-  </si>
-  <si>
-    <t>efficiency_B</t>
-  </si>
-  <si>
-    <t>num_doses_B</t>
-  </si>
-  <si>
-    <t>price_B</t>
-  </si>
-  <si>
-    <t>num_X_B</t>
-  </si>
-  <si>
-    <t>image_title_B</t>
+    <t>efficiency_1</t>
+  </si>
+  <si>
+    <t>num_doses_2</t>
+  </si>
+  <si>
+    <t>num_doses_1</t>
+  </si>
+  <si>
+    <t>price_1</t>
+  </si>
+  <si>
+    <t>num_X_1</t>
+  </si>
+  <si>
+    <t>image_title_1</t>
+  </si>
+  <si>
+    <t>efficiency_2</t>
+  </si>
+  <si>
+    <t>price_2</t>
+  </si>
+  <si>
+    <t>num_X_2</t>
+  </si>
+  <si>
+    <t>image_title_2</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,22 +480,22 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
included instructions and TrialPage.html
</commit_message>
<xml_diff>
--- a/pilot_2_projects/static/Parameters.xlsx
+++ b/pilot_2_projects/static/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frauke/GithubRepoTree/pilot_2_projects/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A626F5C-61E6-F54C-AE3A-9425D62EF12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20E5B4C-F5AE-DA4C-B633-8A4E9BB7385F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AD373C2C-5915-3449-9931-3E1FB904DA92}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>matrix_60.png</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>image_title_2</t>
+  </si>
+  <si>
+    <t>comparison</t>
+  </si>
+  <si>
+    <t>comparable efficiency</t>
+  </si>
+  <si>
+    <t>pure cost effect</t>
+  </si>
+  <si>
+    <t>sanity check</t>
+  </si>
+  <si>
+    <t>same efficiency</t>
   </si>
 </sst>
 </file>
@@ -467,15 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CB44EE-A13A-B449-954A-F65A63BC6646}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -506,86 +521,95 @@
       <c r="J1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1">
+        <v>320</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1.5</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>2.125</v>
-      </c>
-      <c r="G2" s="1">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1">
-        <v>340</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="F3" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="G3" s="1">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1">
+        <v>280</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
         <v>80</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>32</v>
-      </c>
-      <c r="H3" s="1">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1">
-        <v>320</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
       </c>
       <c r="F4" s="1">
         <v>1.875</v>
@@ -602,176 +626,194 @@
       <c r="J4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1">
+        <v>320</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
         <v>120</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="3">
-        <v>1.75</v>
-      </c>
-      <c r="G5" s="1">
-        <v>28</v>
-      </c>
-      <c r="H5" s="1">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1">
-        <v>280</v>
-      </c>
-      <c r="J5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="F6">
+        <v>2.125</v>
+      </c>
+      <c r="G6" s="1">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1">
+        <v>340</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>2.5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
         <v>100</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <v>0.625</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G7" s="1">
         <v>10</v>
       </c>
-      <c r="H6" s="1">
-        <v>16</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H7" s="1">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1">
         <v>100</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>20</v>
       </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
         <v>200</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <v>1.25</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G8" s="1">
         <v>20</v>
       </c>
-      <c r="H7" s="2">
-        <v>16</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H8" s="2">
+        <v>16</v>
+      </c>
+      <c r="I8" s="1">
         <v>200</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>7.5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>30</v>
       </c>
-      <c r="C8" s="1">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
         <v>300</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F9" s="1">
         <v>1.875</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G9" s="1">
         <v>30</v>
       </c>
-      <c r="H8" s="2">
-        <v>16</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H9" s="2">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1">
         <v>300</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1">
-        <v>160</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>8</v>
-      </c>
-      <c r="H9" s="1">
-        <v>4</v>
-      </c>
-      <c r="I9" s="1">
-        <v>80</v>
-      </c>
-      <c r="J9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
         <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
         <v>160</v>
@@ -783,16 +825,54 @@
         <v>2</v>
       </c>
       <c r="G10" s="1">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1">
+        <v>80</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <v>160</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
         <v>32</v>
       </c>
-      <c r="H10" s="1">
-        <v>16</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="H11" s="1">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1">
         <v>320</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>8</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>